<commit_message>
Update post quiz result
</commit_message>
<xml_diff>
--- a/src/main/resources/sample_data.xlsx
+++ b/src/main/resources/sample_data.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18828"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{91BF8A2C-B08D-48CB-B17D-344100EBFEED}" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{053F066B-1806-441A-96DA-05C45FE4D1E1}" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="18">
   <si>
     <t>When was the Civil War 1?</t>
   </si>
@@ -48,6 +48,27 @@
   </si>
   <si>
     <t>Samuel Adams</t>
+  </si>
+  <si>
+    <t>When was the Civil War 3?</t>
+  </si>
+  <si>
+    <t>When was the Civil War 4?</t>
+  </si>
+  <si>
+    <t>When was the Civil War 5?</t>
+  </si>
+  <si>
+    <t>When was the Civil War 6?</t>
+  </si>
+  <si>
+    <t>When was the Civil War 7?</t>
+  </si>
+  <si>
+    <t>When was the Civil War 8?</t>
+  </si>
+  <si>
+    <t>`</t>
   </si>
 </sst>
 </file>
@@ -396,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -521,6 +542,256 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1941</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1942</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1943</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <v>1944</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1941</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1942</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1943</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2">
+        <v>1944</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1941</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1942</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1943</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2">
+        <v>1944</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1941</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1942</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1943</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2">
+        <v>1944</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1941</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1942</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2">
+        <v>1943</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2">
+        <v>1944</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1941</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1942</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1943</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2">
+        <v>1944</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Implement marking quiz functionality.
</commit_message>
<xml_diff>
--- a/src/main/resources/sample_data.xlsx
+++ b/src/main/resources/sample_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18828"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{053F066B-1806-441A-96DA-05C45FE4D1E1}" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{192466E4-83E1-41C5-AEA3-F03208CBCB0A}" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="17">
   <si>
     <t>When was the Civil War 1?</t>
   </si>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>When was the Civil War 8?</t>
-  </si>
-  <si>
-    <t>`</t>
   </si>
 </sst>
 </file>
@@ -417,15 +414,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="38.85546875" customWidth="1"/>
+    <col min="1" max="1" width="47.140625" customWidth="1"/>
     <col min="2" max="3" width="9.140625" style="1"/>
     <col min="4" max="4" width="12.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="1"/>
@@ -787,11 +784,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>